<commit_message>
First Commmit by santosh
</commit_message>
<xml_diff>
--- a/TestNG_Project/Resources/Results.xlsx
+++ b/TestNG_Project/Resources/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Sr No</t>
   </si>
@@ -64,15 +64,6 @@
   </si>
   <si>
     <t>Pratik@123</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -97,32 +88,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,14 +109,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -445,9 +411,6 @@
       <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="0">
@@ -459,9 +422,6 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="2">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="0">
@@ -473,9 +433,6 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="3">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="0">
@@ -487,9 +444,6 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="4">
-        <v>15</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="0">
@@ -501,9 +455,6 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="5">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="0">
@@ -514,9 +465,6 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s" s="6">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>